<commit_message>
new screening + some updates
</commit_message>
<xml_diff>
--- a/Business - Technology Services/DUOL.xlsx
+++ b/Business - Technology Services/DUOL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Business - Technology Services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF8742-5C44-436F-8610-16057790D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA95467-72E1-4DB9-98B9-73A7A9D3D530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="105" windowWidth="14340" windowHeight="15075" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1691,7 +1691,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1846,6 +1846,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1903,10 +1906,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6525,40 +6524,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>Less than -27,00%</c:v>
+                  <c:v>Less than -26,96%</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-27,00% to -21,48%</c:v>
+                  <c:v>-26,96% to -21,43%</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-21,48% to -15,95%</c:v>
+                  <c:v>-21,43% to -15,89%</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-15,95% to -10,42%</c:v>
+                  <c:v>-15,89% to -10,36%</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-10,42% to -4,90%</c:v>
+                  <c:v>-10,36% to -4,83%</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4,90% to 0,63%</c:v>
+                  <c:v>-4,83% to 0,70%</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0,63% to 6,15%</c:v>
+                  <c:v>0,70% to 6,23%</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6,15% to 11,68%</c:v>
+                  <c:v>6,23% to 11,77%</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11,68% to 17,21%</c:v>
+                  <c:v>11,77% to 17,30%</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17,21% to 22,73%</c:v>
+                  <c:v>17,30% to 22,83%</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22,73% to 28,26%</c:v>
+                  <c:v>22,83% to 28,36%</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Greater than 28,26%</c:v>
+                  <c:v>Greater than 28,36%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6585,13 +6584,13 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5</c:v>
@@ -13100,9 +13099,9 @@
       <c r="E17" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="128"/>
-      <c r="M17" s="129"/>
-      <c r="N17" s="130"/>
+      <c r="L17" s="129"/>
+      <c r="M17" s="130"/>
+      <c r="N17" s="131"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -13112,9 +13111,9 @@
         <f>C14/(C16*100)</f>
         <v>0.7151219593242385</v>
       </c>
-      <c r="L18" s="131"/>
-      <c r="M18" s="132"/>
-      <c r="N18" s="133"/>
+      <c r="L18" s="132"/>
+      <c r="M18" s="133"/>
+      <c r="N18" s="134"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
@@ -13124,9 +13123,9 @@
         <f>C15/(C17*100)</f>
         <v>1.042891959394135</v>
       </c>
-      <c r="L19" s="131"/>
-      <c r="M19" s="132"/>
-      <c r="N19" s="133"/>
+      <c r="L19" s="132"/>
+      <c r="M19" s="133"/>
+      <c r="N19" s="134"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -13136,9 +13135,9 @@
         <f>Model!H9/Model!G8-1</f>
         <v>0.36942771084337345</v>
       </c>
-      <c r="L20" s="131"/>
-      <c r="M20" s="132"/>
-      <c r="N20" s="133"/>
+      <c r="L20" s="132"/>
+      <c r="M20" s="133"/>
+      <c r="N20" s="134"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
@@ -13148,9 +13147,9 @@
         <f>Model!I9/Model!H9-1</f>
         <v>0.26894314307709233</v>
       </c>
-      <c r="L21" s="131"/>
-      <c r="M21" s="132"/>
-      <c r="N21" s="133"/>
+      <c r="L21" s="132"/>
+      <c r="M21" s="133"/>
+      <c r="N21" s="134"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
@@ -13160,9 +13159,9 @@
         <f>Model!G14</f>
         <v>-13.167999999999893</v>
       </c>
-      <c r="L22" s="131"/>
-      <c r="M22" s="132"/>
-      <c r="N22" s="133"/>
+      <c r="L22" s="132"/>
+      <c r="M22" s="133"/>
+      <c r="N22" s="134"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
@@ -13172,9 +13171,9 @@
         <f>Model!G17</f>
         <v>17.868000000000109</v>
       </c>
-      <c r="L23" s="131"/>
-      <c r="M23" s="132"/>
-      <c r="N23" s="133"/>
+      <c r="L23" s="132"/>
+      <c r="M23" s="133"/>
+      <c r="N23" s="134"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -13184,9 +13183,9 @@
         <f>Model!G23</f>
         <v>0.73248305722891571</v>
       </c>
-      <c r="L24" s="131"/>
-      <c r="M24" s="132"/>
-      <c r="N24" s="133"/>
+      <c r="L24" s="132"/>
+      <c r="M24" s="133"/>
+      <c r="N24" s="134"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
@@ -13196,9 +13195,9 @@
         <f>Model!G24</f>
         <v>3.0417921686747187E-2</v>
       </c>
-      <c r="L25" s="131"/>
-      <c r="M25" s="132"/>
-      <c r="N25" s="133"/>
+      <c r="L25" s="132"/>
+      <c r="M25" s="133"/>
+      <c r="N25" s="134"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -13208,9 +13207,9 @@
         <f>C12/C23</f>
         <v>455.13782947615573</v>
       </c>
-      <c r="L26" s="131"/>
-      <c r="M26" s="132"/>
-      <c r="N26" s="133"/>
+      <c r="L26" s="132"/>
+      <c r="M26" s="133"/>
+      <c r="N26" s="134"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
@@ -13222,9 +13221,9 @@
       <c r="E27" t="s">
         <v>77</v>
       </c>
-      <c r="L27" s="131"/>
-      <c r="M27" s="132"/>
-      <c r="N27" s="133"/>
+      <c r="L27" s="132"/>
+      <c r="M27" s="133"/>
+      <c r="N27" s="134"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -13233,9 +13232,9 @@
       <c r="C28" s="36">
         <v>0</v>
       </c>
-      <c r="L28" s="134"/>
-      <c r="M28" s="135"/>
-      <c r="N28" s="136"/>
+      <c r="L28" s="135"/>
+      <c r="M28" s="136"/>
+      <c r="N28" s="137"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
@@ -14421,10 +14420,10 @@
       <c r="Q22" s="51"/>
       <c r="R22" s="51"/>
       <c r="S22" s="51"/>
-      <c r="T22" s="148"/>
-      <c r="U22" s="148"/>
-      <c r="V22" s="148"/>
-      <c r="W22" s="147"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="128"/>
       <c r="X22" s="50">
         <v>0.27</v>
       </c>
@@ -25335,10 +25334,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366AC5E7-7FF6-4287-9F23-7D3A6FE15A5F}">
-  <dimension ref="A1:M144"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25366,25 +25365,25 @@
       <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="137" t="s">
+      <c r="H1" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="140"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12">
-        <v>45397</v>
+        <v>45404</v>
       </c>
       <c r="C2" s="18">
-        <v>194.66000399999999</v>
-      </c>
-      <c r="D2">
+        <v>216.38</v>
+      </c>
+      <c r="D2" s="126">
         <f>C2/C3-1</f>
-        <v>-7.7615568343958441E-2</v>
+        <v>0.11157914082853915</v>
       </c>
       <c r="H2" s="61"/>
       <c r="I2" s="62"/>
@@ -25395,14 +25394,14 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
-        <v>45390</v>
+        <v>45397</v>
       </c>
       <c r="C3" s="18">
-        <v>211.03999300000001</v>
-      </c>
-      <c r="D3">
+        <v>194.66000399999999</v>
+      </c>
+      <c r="D3" s="126">
         <f t="shared" ref="D3:D66" si="0">C3/C4-1</f>
-        <v>-1.8464267207670915E-2</v>
+        <v>-7.7615568343958441E-2</v>
       </c>
       <c r="H3" s="64" t="s">
         <v>95</v>
@@ -25425,22 +25424,22 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="12">
-        <v>45383</v>
+        <v>45390</v>
       </c>
       <c r="C4" s="18">
-        <v>215.009995</v>
-      </c>
-      <c r="D4">
+        <v>211.03999300000001</v>
+      </c>
+      <c r="D4" s="126">
         <f t="shared" si="0"/>
-        <v>-2.5251640898978689E-2</v>
+        <v>-1.8464267207670915E-2</v>
       </c>
       <c r="H4" s="69">
         <f>$I$19-3*$I$23</f>
-        <v>-0.27002958446094699</v>
+        <v>-0.26958302426293923</v>
       </c>
       <c r="I4" s="70">
         <f>H4</f>
-        <v>-0.27002958446094699</v>
+        <v>-0.26958302426293923</v>
       </c>
       <c r="J4" s="71">
         <f>COUNTIF(D:D,"&lt;="&amp;H4)</f>
@@ -25448,7 +25447,7 @@
       </c>
       <c r="K4" s="71" t="str">
         <f>"Less than "&amp;TEXT(H4,"0,00%")</f>
-        <v>Less than -27,00%</v>
+        <v>Less than -26,96%</v>
       </c>
       <c r="L4" s="72">
         <f>J4/$I$31</f>
@@ -25461,22 +25460,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
-        <v>45376</v>
+        <v>45383</v>
       </c>
       <c r="C5" s="18">
-        <v>220.58000200000001</v>
-      </c>
-      <c r="D5">
+        <v>215.009995</v>
+      </c>
+      <c r="D5" s="126">
         <f t="shared" si="0"/>
-        <v>-4.9592805370206494E-2</v>
+        <v>-2.5251640898978689E-2</v>
       </c>
       <c r="H5" s="74">
         <f>$I$19-2.4*$I$23</f>
-        <v>-0.2147683314947211</v>
+        <v>-0.21426380716784171</v>
       </c>
       <c r="I5" s="75">
         <f>H5</f>
-        <v>-0.2147683314947211</v>
+        <v>-0.21426380716784171</v>
       </c>
       <c r="J5" s="76">
         <f>COUNTIFS(D:D,"&lt;="&amp;H5,D:D,"&gt;"&amp;H4)</f>
@@ -25484,7 +25483,7 @@
       </c>
       <c r="K5" s="77" t="str">
         <f t="shared" ref="K5:K14" si="1">TEXT(H4,"0,00%")&amp;" to "&amp;TEXT(H5,"0,00%")</f>
-        <v>-27,00% to -21,48%</v>
+        <v>-26,96% to -21,43%</v>
       </c>
       <c r="L5" s="78">
         <f>J5/$I$31</f>
@@ -25497,22 +25496,22 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
-        <v>45369</v>
+        <v>45376</v>
       </c>
       <c r="C6" s="18">
-        <v>232.08999600000001</v>
-      </c>
-      <c r="D6">
+        <v>220.58000200000001</v>
+      </c>
+      <c r="D6" s="126">
         <f t="shared" si="0"/>
-        <v>7.2802072160526476E-2</v>
+        <v>-4.9592805370206494E-2</v>
       </c>
       <c r="H6" s="74">
         <f>$I$19-1.8*$I$23</f>
-        <v>-0.15950707852849527</v>
+        <v>-0.15894459007274417</v>
       </c>
       <c r="I6" s="75">
         <f t="shared" ref="I6:I14" si="2">H6</f>
-        <v>-0.15950707852849527</v>
+        <v>-0.15894459007274417</v>
       </c>
       <c r="J6" s="76">
         <f t="shared" ref="J6:J14" si="3">COUNTIFS(D:D,"&lt;="&amp;H6,D:D,"&gt;"&amp;H5)</f>
@@ -25520,35 +25519,35 @@
       </c>
       <c r="K6" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>-21,48% to -15,95%</v>
+        <v>-21,43% to -15,89%</v>
       </c>
       <c r="L6" s="78">
         <f t="shared" ref="L6:L15" si="4">J6/$I$31</f>
-        <v>1.4084507042253521E-2</v>
+        <v>1.3986013986013986E-2</v>
       </c>
       <c r="M6" s="79">
         <f t="shared" ref="M6:M15" si="5">M5+L6</f>
-        <v>1.4084507042253521E-2</v>
+        <v>1.3986013986013986E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
-        <v>45362</v>
+        <v>45369</v>
       </c>
       <c r="C7" s="18">
-        <v>216.33999600000001</v>
-      </c>
-      <c r="D7">
+        <v>232.08999600000001</v>
+      </c>
+      <c r="D7" s="126">
         <f t="shared" si="0"/>
-        <v>1.3159729373669826E-2</v>
+        <v>7.2802072160526476E-2</v>
       </c>
       <c r="H7" s="74">
         <f>$I$19-1.2*$I$23</f>
-        <v>-0.10424582556226938</v>
+        <v>-0.10362537297764662</v>
       </c>
       <c r="I7" s="75">
         <f t="shared" si="2"/>
-        <v>-0.10424582556226938</v>
+        <v>-0.10362537297764662</v>
       </c>
       <c r="J7" s="76">
         <f t="shared" si="3"/>
@@ -25556,35 +25555,35 @@
       </c>
       <c r="K7" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>-15,95% to -10,42%</v>
+        <v>-15,89% to -10,36%</v>
       </c>
       <c r="L7" s="78">
         <f t="shared" si="4"/>
-        <v>5.6338028169014086E-2</v>
+        <v>5.5944055944055944E-2</v>
       </c>
       <c r="M7" s="79">
         <f t="shared" si="5"/>
-        <v>7.0422535211267609E-2</v>
+        <v>6.9930069930069935E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
-        <v>45355</v>
+        <v>45362</v>
       </c>
       <c r="C8" s="18">
-        <v>213.529999</v>
-      </c>
-      <c r="D8">
+        <v>216.33999600000001</v>
+      </c>
+      <c r="D8" s="126">
         <f t="shared" si="0"/>
-        <v>-9.7086580889539031E-2</v>
+        <v>1.3159729373669826E-2</v>
       </c>
       <c r="H8" s="74">
         <f>$I$19-0.6*$I$23</f>
-        <v>-4.8984572596043538E-2</v>
+        <v>-4.8306155882549093E-2</v>
       </c>
       <c r="I8" s="75">
         <f t="shared" si="2"/>
-        <v>-4.8984572596043538E-2</v>
+        <v>-4.8306155882549093E-2</v>
       </c>
       <c r="J8" s="76">
         <f t="shared" si="3"/>
@@ -25592,143 +25591,143 @@
       </c>
       <c r="K8" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>-10,42% to -4,90%</v>
+        <v>-10,36% to -4,83%</v>
       </c>
       <c r="L8" s="78">
         <f t="shared" si="4"/>
-        <v>0.16901408450704225</v>
+        <v>0.16783216783216784</v>
       </c>
       <c r="M8" s="79">
         <f t="shared" si="5"/>
-        <v>0.23943661971830987</v>
+        <v>0.23776223776223776</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
+        <v>45355</v>
+      </c>
+      <c r="C9" s="18">
+        <v>213.529999</v>
+      </c>
+      <c r="D9" s="126">
+        <f t="shared" si="0"/>
+        <v>-9.7086580889539031E-2</v>
+      </c>
+      <c r="H9" s="74">
+        <f>$I$19</f>
+        <v>7.0130612125484468E-3</v>
+      </c>
+      <c r="I9" s="75">
+        <f t="shared" si="2"/>
+        <v>7.0130612125484468E-3</v>
+      </c>
+      <c r="J9" s="76">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="K9" s="77" t="str">
+        <f t="shared" si="1"/>
+        <v>-4,83% to 0,70%</v>
+      </c>
+      <c r="L9" s="78">
+        <f t="shared" si="4"/>
+        <v>0.30069930069930068</v>
+      </c>
+      <c r="M9" s="79">
+        <f t="shared" si="5"/>
+        <v>0.53846153846153844</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
         <v>45348</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C10" s="18">
         <v>236.490005</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="126">
         <f t="shared" si="0"/>
         <v>0.33512108803926233</v>
       </c>
-      <c r="H9" s="74">
-        <f>$I$19</f>
-        <v>6.2766803701823151E-3</v>
-      </c>
-      <c r="I9" s="75">
+      <c r="H10" s="74">
+        <f>$I$19+0.6*$I$23</f>
+        <v>6.2332278307645983E-2</v>
+      </c>
+      <c r="I10" s="75">
         <f t="shared" si="2"/>
-        <v>6.2766803701823151E-3</v>
-      </c>
-      <c r="J9" s="76">
+        <v>6.2332278307645983E-2</v>
+      </c>
+      <c r="J10" s="76">
         <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="K9" s="77" t="str">
+        <v>29</v>
+      </c>
+      <c r="K10" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>-4,90% to 0,63%</v>
-      </c>
-      <c r="L9" s="78">
+        <v>0,70% to 6,23%</v>
+      </c>
+      <c r="L10" s="78">
         <f t="shared" si="4"/>
-        <v>0.29577464788732394</v>
-      </c>
-      <c r="M9" s="79">
+        <v>0.20279720279720279</v>
+      </c>
+      <c r="M10" s="79">
         <f t="shared" si="5"/>
-        <v>0.53521126760563376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+        <v>0.74125874125874125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
         <v>45341</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C11" s="18">
         <v>177.13000500000001</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="126">
         <f t="shared" si="0"/>
         <v>-4.2022656853087703E-2</v>
       </c>
-      <c r="H10" s="74">
-        <f>$I$19+0.6*$I$23</f>
-        <v>6.1537933336408168E-2</v>
-      </c>
-      <c r="I10" s="75">
+      <c r="H11" s="74">
+        <f>$I$19+1.2*$I$23</f>
+        <v>0.11765149540274353</v>
+      </c>
+      <c r="I11" s="75">
         <f t="shared" si="2"/>
-        <v>6.1537933336408168E-2</v>
-      </c>
-      <c r="J10" s="76">
+        <v>0.11765149540274353</v>
+      </c>
+      <c r="J11" s="76">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="K10" s="77" t="str">
+        <v>28</v>
+      </c>
+      <c r="K11" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>0,63% to 6,15%</v>
-      </c>
-      <c r="L10" s="78">
+        <v>6,23% to 11,77%</v>
+      </c>
+      <c r="L11" s="78">
         <f t="shared" si="4"/>
-        <v>0.21126760563380281</v>
-      </c>
-      <c r="M10" s="79">
+        <v>0.19580419580419581</v>
+      </c>
+      <c r="M11" s="79">
         <f t="shared" si="5"/>
-        <v>0.74647887323943651</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+        <v>0.93706293706293708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
         <v>45334</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C12" s="18">
         <v>184.89999399999999</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="126">
         <f t="shared" si="0"/>
         <v>-3.5673364043147915E-2</v>
       </c>
-      <c r="H11" s="74">
-        <f>$I$19+1.2*$I$23</f>
-        <v>0.11679918630263403</v>
-      </c>
-      <c r="I11" s="75">
-        <f t="shared" si="2"/>
-        <v>0.11679918630263403</v>
-      </c>
-      <c r="J11" s="76">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="K11" s="77" t="str">
-        <f t="shared" si="1"/>
-        <v>6,15% to 11,68%</v>
-      </c>
-      <c r="L11" s="78">
-        <f t="shared" si="4"/>
-        <v>0.19014084507042253</v>
-      </c>
-      <c r="M11" s="79">
-        <f t="shared" si="5"/>
-        <v>0.93661971830985902</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
-        <v>45327</v>
-      </c>
-      <c r="C12" s="18">
-        <v>191.740005</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>7.1831885917781335E-2</v>
-      </c>
       <c r="H12" s="74">
         <f>$I$19+1.8*$I$23</f>
-        <v>0.17206043926885989</v>
+        <v>0.17297071249784104</v>
       </c>
       <c r="I12" s="75">
         <f t="shared" si="2"/>
-        <v>0.17206043926885989</v>
+        <v>0.17297071249784104</v>
       </c>
       <c r="J12" s="76">
         <f t="shared" si="3"/>
@@ -25736,35 +25735,35 @@
       </c>
       <c r="K12" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>11,68% to 17,21%</v>
+        <v>11,77% to 17,30%</v>
       </c>
       <c r="L12" s="78">
         <f t="shared" si="4"/>
-        <v>3.5211267605633804E-2</v>
+        <v>3.4965034965034968E-2</v>
       </c>
       <c r="M12" s="79">
         <f t="shared" si="5"/>
-        <v>0.97183098591549277</v>
+        <v>0.97202797202797209</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
-        <v>45320</v>
+        <v>45327</v>
       </c>
       <c r="C13" s="18">
-        <v>178.88999899999999</v>
-      </c>
-      <c r="D13">
+        <v>191.740005</v>
+      </c>
+      <c r="D13" s="126">
         <f t="shared" si="0"/>
-        <v>-7.2580227448702517E-2</v>
+        <v>7.1831885917781335E-2</v>
       </c>
       <c r="H13" s="74">
         <f>$I$19+2.4*$I$23</f>
-        <v>0.22732169223508572</v>
+        <v>0.22828992959293859</v>
       </c>
       <c r="I13" s="75">
         <f t="shared" si="2"/>
-        <v>0.22732169223508572</v>
+        <v>0.22828992959293859</v>
       </c>
       <c r="J13" s="76">
         <f t="shared" si="3"/>
@@ -25772,7 +25771,7 @@
       </c>
       <c r="K13" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>17,21% to 22,73%</v>
+        <v>17,30% to 22,83%</v>
       </c>
       <c r="L13" s="78">
         <f t="shared" si="4"/>
@@ -25780,27 +25779,27 @@
       </c>
       <c r="M13" s="79">
         <f t="shared" si="5"/>
-        <v>0.97183098591549277</v>
+        <v>0.97202797202797209</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
-        <v>45313</v>
+        <v>45320</v>
       </c>
       <c r="C14" s="18">
-        <v>192.88999899999999</v>
-      </c>
-      <c r="D14">
+        <v>178.88999899999999</v>
+      </c>
+      <c r="D14" s="126">
         <f t="shared" si="0"/>
-        <v>-8.7872916098472587E-3</v>
+        <v>-7.2580227448702517E-2</v>
       </c>
       <c r="H14" s="74">
         <f>$I$19+3*$I$23</f>
-        <v>0.28258294520131161</v>
+        <v>0.28360914668803616</v>
       </c>
       <c r="I14" s="75">
         <f t="shared" si="2"/>
-        <v>0.28258294520131161</v>
+        <v>0.28360914668803616</v>
       </c>
       <c r="J14" s="76">
         <f t="shared" si="3"/>
@@ -25808,7 +25807,7 @@
       </c>
       <c r="K14" s="77" t="str">
         <f t="shared" si="1"/>
-        <v>22,73% to 28,26%</v>
+        <v>22,83% to 28,36%</v>
       </c>
       <c r="L14" s="78">
         <f t="shared" si="4"/>
@@ -25816,19 +25815,19 @@
       </c>
       <c r="M14" s="79">
         <f t="shared" si="5"/>
-        <v>0.97183098591549277</v>
+        <v>0.97202797202797209</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
-        <v>45306</v>
+        <v>45313</v>
       </c>
       <c r="C15" s="18">
-        <v>194.60000600000001</v>
-      </c>
-      <c r="D15">
+        <v>192.88999899999999</v>
+      </c>
+      <c r="D15" s="126">
         <f t="shared" si="0"/>
-        <v>-8.2118718034968063E-2</v>
+        <v>-8.7872916098472587E-3</v>
       </c>
       <c r="H15" s="80"/>
       <c r="I15" s="81" t="s">
@@ -25840,133 +25839,133 @@
       </c>
       <c r="K15" s="81" t="str">
         <f>"Greater than "&amp;TEXT(H14,"0,00%")</f>
-        <v>Greater than 28,26%</v>
+        <v>Greater than 28,36%</v>
       </c>
       <c r="L15" s="82">
         <f t="shared" si="4"/>
-        <v>2.8169014084507043E-2</v>
+        <v>2.7972027972027972E-2</v>
       </c>
       <c r="M15" s="82">
         <f t="shared" si="5"/>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
+        <v>45306</v>
+      </c>
+      <c r="C16" s="18">
+        <v>194.60000600000001</v>
+      </c>
+      <c r="D16" s="126">
+        <f t="shared" si="0"/>
+        <v>-8.2118718034968063E-2</v>
+      </c>
+      <c r="H16" s="83"/>
+      <c r="M16" s="84"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
         <v>45299</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C17" s="18">
         <v>212.009995</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="126">
         <f t="shared" si="0"/>
         <v>3.857741295165984E-2</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="M16" s="84"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="12">
+      <c r="H17" s="141" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="142"/>
+      <c r="M17" s="84"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
         <v>45292</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C18" s="18">
         <v>204.134995</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="126">
         <f t="shared" si="0"/>
         <v>-0.1001322918192914</v>
       </c>
-      <c r="H17" s="140" t="s">
-        <v>132</v>
-      </c>
-      <c r="I17" s="141"/>
-      <c r="M17" s="84"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
+      <c r="H18" s="143"/>
+      <c r="I18" s="144"/>
+      <c r="M18" s="84"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
         <v>45285</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C19" s="18">
         <v>226.85000600000001</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="126">
         <f t="shared" si="0"/>
         <v>-4.7848873032528827E-2</v>
       </c>
-      <c r="H18" s="142"/>
-      <c r="I18" s="143"/>
-      <c r="M18" s="84"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
+      <c r="H19" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" s="122">
+        <f>AVERAGE(D:D)</f>
+        <v>7.0130612125484468E-3</v>
+      </c>
+      <c r="M19" s="84"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="12">
         <v>45278</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C20" s="18">
         <v>238.25</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="126">
         <f t="shared" si="0"/>
         <v>2.9202103131839241E-2</v>
       </c>
-      <c r="H19" s="85" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" s="122">
-        <f>AVERAGE(D:D)</f>
-        <v>6.2766803701823151E-3</v>
-      </c>
-      <c r="M19" s="84"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
+      <c r="H20" s="85" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="122">
+        <f>_xlfn.STDEV.S(D:D)/SQRT(COUNT(D:D))</f>
+        <v>7.7100422159371634E-3</v>
+      </c>
+      <c r="M20" s="84"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="12">
         <v>45271</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C21" s="18">
         <v>231.490005</v>
       </c>
-      <c r="D20">
+      <c r="D21" s="126">
         <f t="shared" si="0"/>
         <v>7.795112922002323E-2</v>
       </c>
-      <c r="H20" s="85" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="122">
-        <f>_xlfn.STDEV.S(D:D)/SQRT(COUNT(D:D))</f>
-        <v>7.7290355542290589E-3</v>
-      </c>
-      <c r="M20" s="84"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
+      <c r="H21" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="122">
+        <f>MEDIAN(D:D)</f>
+        <v>-7.6949466757081364E-4</v>
+      </c>
+      <c r="M21" s="84"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="12">
         <v>45264</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C22" s="18">
         <v>214.75</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="126">
         <f t="shared" si="0"/>
         <v>6.7979230173755845E-3</v>
-      </c>
-      <c r="H21" s="85" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="122">
-        <f>MEDIAN(D:D)</f>
-        <v>-1.5901968203113626E-3</v>
-      </c>
-      <c r="M21" s="84"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="12">
-        <v>45257</v>
-      </c>
-      <c r="C22" s="18">
-        <v>213.300003</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>-3.6846399991308565E-2</v>
       </c>
       <c r="H22" s="85" t="s">
         <v>105</v>
@@ -25979,94 +25978,94 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
+        <v>45257</v>
+      </c>
+      <c r="C23" s="18">
+        <v>213.300003</v>
+      </c>
+      <c r="D23" s="126">
+        <f t="shared" si="0"/>
+        <v>-3.6846399991308565E-2</v>
+      </c>
+      <c r="H23" s="85" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="122">
+        <f>_xlfn.STDEV.S(D:D)</f>
+        <v>9.2198695158495894E-2</v>
+      </c>
+      <c r="M23" s="84"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
         <v>45250</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C24" s="18">
         <v>221.46000699999999</v>
       </c>
-      <c r="D23">
+      <c r="D24" s="126">
         <f t="shared" si="0"/>
         <v>4.6350169043708922E-2</v>
       </c>
-      <c r="H23" s="85" t="s">
-        <v>106</v>
-      </c>
-      <c r="I23" s="122">
-        <f>_xlfn.STDEV.S(D:D)</f>
-        <v>9.2102088277043095E-2</v>
-      </c>
-      <c r="M23" s="84"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
+      <c r="H24" s="85" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="122">
+        <f>_xlfn.VAR.S(D:D)</f>
+        <v>8.5005993889292544E-3</v>
+      </c>
+      <c r="M24" s="84"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
         <v>45243</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C25" s="18">
         <v>211.64999399999999</v>
       </c>
-      <c r="D24">
+      <c r="D25" s="126">
         <f t="shared" si="0"/>
         <v>5.6727178446203119E-4</v>
       </c>
-      <c r="H24" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="122">
-        <f>_xlfn.VAR.S(D:D)</f>
-        <v>8.4827946649922402E-3</v>
-      </c>
-      <c r="M24" s="84"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="H25" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="123">
+        <f>KURT(D:D)</f>
+        <v>3.5761692065844546</v>
+      </c>
+      <c r="M25" s="84"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="12">
         <v>45236</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C26" s="18">
         <v>211.529999</v>
       </c>
-      <c r="D25">
+      <c r="D26" s="126">
         <f t="shared" si="0"/>
         <v>0.32762189383516094</v>
       </c>
-      <c r="H25" s="85" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" s="123">
-        <f>KURT(D:D)</f>
-        <v>3.6803059267123843</v>
-      </c>
-      <c r="M25" s="84"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
+      <c r="H26" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="123">
+        <f>SKEW(D:D)</f>
+        <v>1.1921520470223386</v>
+      </c>
+      <c r="M26" s="84"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="12">
         <v>45229</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C27" s="18">
         <v>159.33000200000001</v>
       </c>
-      <c r="D26">
+      <c r="D27" s="126">
         <f t="shared" si="0"/>
         <v>0.10977219636131941</v>
-      </c>
-      <c r="H26" s="85" t="s">
-        <v>109</v>
-      </c>
-      <c r="I26" s="123">
-        <f>SKEW(D:D)</f>
-        <v>1.2183112622984311</v>
-      </c>
-      <c r="M26" s="84"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
-        <v>45222</v>
-      </c>
-      <c r="C27" s="18">
-        <v>143.570007</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>-6.548198706365993E-2</v>
       </c>
       <c r="H27" s="85" t="s">
         <v>98</v>
@@ -26079,14 +26078,14 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="12">
-        <v>45215</v>
+        <v>45222</v>
       </c>
       <c r="C28" s="18">
-        <v>153.63000500000001</v>
-      </c>
-      <c r="D28">
+        <v>143.570007</v>
+      </c>
+      <c r="D28" s="126">
         <f t="shared" si="0"/>
-        <v>-4.0412247080115593E-2</v>
+        <v>-6.548198706365993E-2</v>
       </c>
       <c r="H28" s="85" t="s">
         <v>110</v>
@@ -26099,14 +26098,14 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="12">
-        <v>45208</v>
+        <v>45215</v>
       </c>
       <c r="C29" s="18">
-        <v>160.10000600000001</v>
-      </c>
-      <c r="D29">
+        <v>153.63000500000001</v>
+      </c>
+      <c r="D29" s="126">
         <f t="shared" si="0"/>
-        <v>-2.5207007269635651E-2</v>
+        <v>-4.0412247080115593E-2</v>
       </c>
       <c r="H29" s="85" t="s">
         <v>111</v>
@@ -26119,68 +26118,68 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="12">
+        <v>45208</v>
+      </c>
+      <c r="C30" s="18">
+        <v>160.10000600000001</v>
+      </c>
+      <c r="D30" s="126">
+        <f t="shared" si="0"/>
+        <v>-2.5207007269635651E-2</v>
+      </c>
+      <c r="H30" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="123">
+        <f>SUM(D:D)</f>
+        <v>1.0028677533944279</v>
+      </c>
+      <c r="M30" s="84"/>
+    </row>
+    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="12">
         <v>45201</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C31" s="18">
         <v>164.240005</v>
       </c>
-      <c r="D30">
+      <c r="D31" s="126">
         <f t="shared" si="0"/>
         <v>-9.8269129386541199E-3</v>
       </c>
-      <c r="H30" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="I30" s="123">
-        <f>SUM(D:D)</f>
-        <v>0.89128861256588876</v>
-      </c>
-      <c r="M30" s="84"/>
-    </row>
-    <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="12">
+      <c r="H31" s="86" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="63">
+        <f>COUNT(D:D)</f>
+        <v>143</v>
+      </c>
+      <c r="M31" s="84"/>
+    </row>
+    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12">
         <v>45194</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C32" s="18">
         <v>165.86999499999999</v>
       </c>
-      <c r="D31">
+      <c r="D32" s="126">
         <f t="shared" si="0"/>
         <v>8.6460975783860361E-2</v>
       </c>
-      <c r="H31" s="86" t="s">
-        <v>113</v>
-      </c>
-      <c r="I31" s="63">
-        <f>COUNT(D:D)</f>
-        <v>142</v>
-      </c>
-      <c r="M31" s="84"/>
-    </row>
-    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="12">
+      <c r="H32" s="88"/>
+      <c r="M32" s="84"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="12">
         <v>45187</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C33" s="18">
         <v>152.66999799999999</v>
       </c>
-      <c r="D32">
+      <c r="D33" s="126">
         <f t="shared" si="0"/>
         <v>-4.3001322904791195E-2</v>
-      </c>
-      <c r="H32" s="88"/>
-      <c r="M32" s="84"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="12">
-        <v>45180</v>
-      </c>
-      <c r="C33" s="18">
-        <v>159.529999</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>1.929591781023321E-2</v>
       </c>
       <c r="H33" s="89"/>
       <c r="I33" s="90" t="s">
@@ -26199,46 +26198,46 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
+        <v>45180</v>
+      </c>
+      <c r="C34" s="18">
+        <v>159.529999</v>
+      </c>
+      <c r="D34" s="126">
+        <f t="shared" si="0"/>
+        <v>1.929591781023321E-2</v>
+      </c>
+      <c r="H34" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="78">
+        <f>AVERAGEIF(D:D,"&gt;0")</f>
+        <v>7.5861524839146252E-2</v>
+      </c>
+      <c r="J34" s="76">
+        <f>COUNTIF(D:D,"&gt;0")</f>
+        <v>70</v>
+      </c>
+      <c r="K34" s="78">
+        <f>J34/$I$31</f>
+        <v>0.48951048951048953</v>
+      </c>
+      <c r="L34" s="79">
+        <f>K34*I34</f>
+        <v>3.7135012159022644E-2</v>
+      </c>
+      <c r="M34" s="84"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="12">
         <v>45173</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C35" s="18">
         <v>156.509995</v>
       </c>
-      <c r="D34">
+      <c r="D35" s="126">
         <f t="shared" si="0"/>
         <v>5.0966942666760051E-2</v>
-      </c>
-      <c r="H34" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="I34" s="78">
-        <f>AVERAGEIF(D:D,"&gt;0")</f>
-        <v>7.534387823060433E-2</v>
-      </c>
-      <c r="J34" s="76">
-        <f>COUNTIF(D:D,"&gt;0")</f>
-        <v>69</v>
-      </c>
-      <c r="K34" s="78">
-        <f>J34/$I$31</f>
-        <v>0.4859154929577465</v>
-      </c>
-      <c r="L34" s="79">
-        <f>K34*I34</f>
-        <v>3.6610757731772525E-2</v>
-      </c>
-      <c r="M34" s="84"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="12">
-        <v>45166</v>
-      </c>
-      <c r="C35" s="18">
-        <v>148.91999799999999</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>0.10253935205615261</v>
       </c>
       <c r="H35" s="92" t="s">
         <v>118</v>
@@ -26253,24 +26252,24 @@
       </c>
       <c r="K35" s="78">
         <f>J35/$I$31</f>
-        <v>0.5140845070422535</v>
+        <v>0.51048951048951052</v>
       </c>
       <c r="L35" s="79">
         <f t="shared" ref="L35:L36" si="6">K35*I35</f>
-        <v>-3.0334077361590231E-2</v>
+        <v>-3.012195094647422E-2</v>
       </c>
       <c r="M35" s="84"/>
     </row>
     <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12">
-        <v>45159</v>
+        <v>45166</v>
       </c>
       <c r="C36" s="18">
-        <v>135.070007</v>
-      </c>
-      <c r="D36">
+        <v>148.91999799999999</v>
+      </c>
+      <c r="D36" s="126">
         <f t="shared" si="0"/>
-        <v>9.0153388375247889E-2</v>
+        <v>0.10253935205615261</v>
       </c>
       <c r="H36" s="93" t="s">
         <v>119</v>
@@ -26294,14 +26293,14 @@
     </row>
     <row r="37" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="12">
-        <v>45152</v>
+        <v>45159</v>
       </c>
       <c r="C37" s="18">
-        <v>123.900002</v>
-      </c>
-      <c r="D37">
+        <v>135.070007</v>
+      </c>
+      <c r="D37" s="126">
         <f t="shared" si="0"/>
-        <v>-0.10741298332127347</v>
+        <v>9.0153388375247889E-2</v>
       </c>
       <c r="H37" s="88"/>
       <c r="I37" s="95"/>
@@ -26312,55 +26311,55 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="12">
+        <v>45152</v>
+      </c>
+      <c r="C38" s="18">
+        <v>123.900002</v>
+      </c>
+      <c r="D38" s="126">
+        <f t="shared" si="0"/>
+        <v>-0.10741298332127347</v>
+      </c>
+      <c r="H38" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="I38" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="J38" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="K38" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="L38" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="M38" s="91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
         <v>45145</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C39" s="18">
         <v>138.80999800000001</v>
       </c>
-      <c r="D38">
+      <c r="D39" s="126">
         <f t="shared" si="0"/>
         <v>1.0556180761821521E-2</v>
       </c>
-      <c r="H38" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="I38" s="90" t="s">
-        <v>121</v>
-      </c>
-      <c r="J38" s="90" t="s">
-        <v>122</v>
-      </c>
-      <c r="K38" s="90" t="s">
-        <v>123</v>
-      </c>
-      <c r="L38" s="90" t="s">
-        <v>124</v>
-      </c>
-      <c r="M38" s="91" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
-        <v>45138</v>
-      </c>
-      <c r="C39" s="18">
-        <v>137.36000100000001</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>-9.0090125658247922E-2</v>
-      </c>
       <c r="H39" s="96">
         <v>1</v>
       </c>
       <c r="I39" s="78">
         <f>$I$19+($H39*$I$23)</f>
-        <v>9.8378768647225417E-2</v>
+        <v>9.9211756371044346E-2</v>
       </c>
       <c r="J39" s="78">
         <f>$I$19-($H39*$I$23)</f>
-        <v>-8.5825407906860773E-2</v>
+        <v>-8.5185633945947442E-2</v>
       </c>
       <c r="K39" s="76">
         <f>COUNTIFS(D:D,"&lt;"&amp;I39,D:D,"&gt;"&amp;J39)</f>
@@ -26368,7 +26367,7 @@
       </c>
       <c r="L39" s="78">
         <f>K39/$I$31</f>
-        <v>0.76760563380281688</v>
+        <v>0.76223776223776218</v>
       </c>
       <c r="M39" s="79">
         <v>0.68269999999999997</v>
@@ -26376,552 +26375,552 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="12">
+        <v>45138</v>
+      </c>
+      <c r="C40" s="18">
+        <v>137.36000100000001</v>
+      </c>
+      <c r="D40" s="126">
+        <f t="shared" si="0"/>
+        <v>-9.0090125658247922E-2</v>
+      </c>
+      <c r="H40" s="96">
+        <v>2</v>
+      </c>
+      <c r="I40" s="78">
+        <f>$I$19+($H40*$I$23)</f>
+        <v>0.19141045152954023</v>
+      </c>
+      <c r="J40" s="78">
+        <f>$I$19-($H40*$I$23)</f>
+        <v>-0.17738432910444335</v>
+      </c>
+      <c r="K40" s="76">
+        <f>COUNTIFS(D:D,"&lt;"&amp;I40,D:D,"&gt;"&amp;J40)</f>
+        <v>137</v>
+      </c>
+      <c r="L40" s="78">
+        <f>K40/$I$31</f>
+        <v>0.95804195804195802</v>
+      </c>
+      <c r="M40" s="79">
+        <v>0.95450000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="12">
         <v>45131</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C41" s="18">
         <v>150.96000699999999</v>
       </c>
-      <c r="D40">
+      <c r="D41" s="126">
         <f t="shared" si="0"/>
         <v>9.7659331103678859E-3</v>
       </c>
-      <c r="H40" s="96">
-        <v>2</v>
-      </c>
-      <c r="I40" s="78">
-        <f>$I$19+($H40*$I$23)</f>
-        <v>0.1904808569242685</v>
-      </c>
-      <c r="J40" s="78">
-        <f>$I$19-($H40*$I$23)</f>
-        <v>-0.17792749618390388</v>
-      </c>
-      <c r="K40" s="76">
-        <f>COUNTIFS(D:D,"&lt;"&amp;I40,D:D,"&gt;"&amp;J40)</f>
-        <v>136</v>
-      </c>
-      <c r="L40" s="78">
-        <f>K40/$I$31</f>
-        <v>0.95774647887323938</v>
-      </c>
-      <c r="M40" s="79">
-        <v>0.95450000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="12">
+      <c r="H41" s="96">
+        <v>3</v>
+      </c>
+      <c r="I41" s="78">
+        <f>$I$19+($H41*$I$23)</f>
+        <v>0.28360914668803616</v>
+      </c>
+      <c r="J41" s="78">
+        <f>$I$19-($H41*$I$23)</f>
+        <v>-0.26958302426293923</v>
+      </c>
+      <c r="K41" s="76">
+        <f>COUNTIFS(D:D,"&lt;"&amp;I41,D:D,"&gt;"&amp;J41)</f>
+        <v>139</v>
+      </c>
+      <c r="L41" s="78">
+        <f>K41/$I$31</f>
+        <v>0.97202797202797198</v>
+      </c>
+      <c r="M41" s="97">
+        <v>0.99729999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="12">
         <v>45124</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C42" s="18">
         <v>149.5</v>
       </c>
-      <c r="D41">
+      <c r="D42" s="126">
         <f t="shared" si="0"/>
         <v>-6.6851717840044067E-5</v>
       </c>
-      <c r="H41" s="96">
-        <v>3</v>
-      </c>
-      <c r="I41" s="78">
-        <f>$I$19+($H41*$I$23)</f>
-        <v>0.28258294520131161</v>
-      </c>
-      <c r="J41" s="78">
-        <f>$I$19-($H41*$I$23)</f>
-        <v>-0.27002958446094699</v>
-      </c>
-      <c r="K41" s="76">
-        <f>COUNTIFS(D:D,"&lt;"&amp;I41,D:D,"&gt;"&amp;J41)</f>
-        <v>138</v>
-      </c>
-      <c r="L41" s="78">
-        <f>K41/$I$31</f>
-        <v>0.971830985915493</v>
-      </c>
-      <c r="M41" s="97">
-        <v>0.99729999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="12">
+      <c r="H42" s="74"/>
+      <c r="M42" s="97"/>
+    </row>
+    <row r="43" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="12">
         <v>45117</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C43" s="18">
         <v>149.509995</v>
       </c>
-      <c r="D42">
+      <c r="D43" s="126">
         <f t="shared" si="0"/>
         <v>0.1054343438077634</v>
       </c>
-      <c r="H42" s="74"/>
-      <c r="M42" s="97"/>
-    </row>
-    <row r="43" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="12">
+      <c r="H43" s="145" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="146"/>
+      <c r="J43" s="146"/>
+      <c r="K43" s="146"/>
+      <c r="L43" s="146"/>
+      <c r="M43" s="147"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="12">
         <v>45110</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C44" s="18">
         <v>135.25</v>
       </c>
-      <c r="D43">
+      <c r="D44" s="126">
         <f t="shared" si="0"/>
         <v>-5.3798809937053105E-2</v>
       </c>
-      <c r="H43" s="144" t="s">
-        <v>126</v>
-      </c>
-      <c r="I43" s="145"/>
-      <c r="J43" s="145"/>
-      <c r="K43" s="145"/>
-      <c r="L43" s="145"/>
-      <c r="M43" s="146"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="12">
+      <c r="H44" s="98">
+        <v>0.01</v>
+      </c>
+      <c r="I44" s="99">
+        <f t="shared" ref="I44:I58" si="7">_xlfn.PERCENTILE.INC(D:D,H44)</f>
+        <v>-0.17625708598154247</v>
+      </c>
+      <c r="J44" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="K44" s="99">
+        <f t="shared" ref="K44:K56" si="8">_xlfn.PERCENTILE.INC(D:D,J44)</f>
+        <v>-6.5532251052551671E-2</v>
+      </c>
+      <c r="L44" s="100">
+        <v>0.85</v>
+      </c>
+      <c r="M44" s="101">
+        <f t="shared" ref="M44:M58" si="9">_xlfn.PERCENTILE.INC(D:D,L44)</f>
+        <v>7.790344746207456E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="12">
         <v>45103</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C45" s="18">
         <v>142.94000199999999</v>
       </c>
-      <c r="D44">
+      <c r="D45" s="126">
         <f t="shared" si="0"/>
         <v>2.0781282730709671E-2</v>
       </c>
-      <c r="H44" s="98">
-        <v>0.01</v>
-      </c>
-      <c r="I44" s="99">
-        <f t="shared" ref="I44:I58" si="7">_xlfn.PERCENTILE.INC(D:D,H44)</f>
-        <v>-0.17669293733481406</v>
-      </c>
-      <c r="J44" s="100">
-        <v>0.2</v>
-      </c>
-      <c r="K44" s="99">
-        <f t="shared" ref="K44:K56" si="8">_xlfn.PERCENTILE.INC(D:D,J44)</f>
-        <v>-6.5549005715515585E-2</v>
-      </c>
-      <c r="L44" s="100">
-        <v>0.85</v>
-      </c>
-      <c r="M44" s="101">
-        <f t="shared" ref="M44:M58" si="9">_xlfn.PERCENTILE.INC(D:D,L44)</f>
-        <v>7.7241518117892066E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="12">
+      <c r="H45" s="102">
+        <v>0.02</v>
+      </c>
+      <c r="I45" s="103">
+        <f t="shared" si="7"/>
+        <v>-0.14870136684728594</v>
+      </c>
+      <c r="J45" s="104">
+        <v>0.25</v>
+      </c>
+      <c r="K45" s="103">
+        <f t="shared" si="8"/>
+        <v>-4.6407647425667942E-2</v>
+      </c>
+      <c r="L45" s="104">
+        <v>0.86</v>
+      </c>
+      <c r="M45" s="105">
+        <f t="shared" si="9"/>
+        <v>8.1363249329655496E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="12">
         <v>45096</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C46" s="18">
         <v>140.029999</v>
       </c>
-      <c r="D45">
+      <c r="D46" s="126">
         <f t="shared" si="0"/>
         <v>-8.3513283491020274E-2</v>
       </c>
-      <c r="H45" s="102">
-        <v>0.02</v>
-      </c>
-      <c r="I45" s="103">
+      <c r="H46" s="102">
+        <v>0.03</v>
+      </c>
+      <c r="I46" s="103">
         <f t="shared" si="7"/>
-        <v>-0.14875556543405979</v>
-      </c>
-      <c r="J45" s="104">
-        <v>0.25</v>
-      </c>
-      <c r="K45" s="103">
+        <v>-0.1228585611805046</v>
+      </c>
+      <c r="J46" s="104">
+        <v>0.3</v>
+      </c>
+      <c r="K46" s="103">
         <f t="shared" si="8"/>
-        <v>-4.6729972435567868E-2</v>
-      </c>
-      <c r="L45" s="104">
-        <v>0.86</v>
-      </c>
-      <c r="M45" s="105">
+        <v>-4.0049487554004413E-2</v>
+      </c>
+      <c r="L46" s="104">
+        <v>0.87</v>
+      </c>
+      <c r="M46" s="105">
         <f t="shared" si="9"/>
-        <v>7.8657542874242176E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="12">
+        <v>8.8454878583209648E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="12">
         <v>45089</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C47" s="18">
         <v>152.78999300000001</v>
       </c>
-      <c r="D46">
+      <c r="D47" s="126">
         <f t="shared" si="0"/>
         <v>-1.9445603028371061E-2</v>
       </c>
-      <c r="H46" s="102">
-        <v>0.03</v>
-      </c>
-      <c r="I46" s="103">
+      <c r="H47" s="102">
+        <v>0.04</v>
+      </c>
+      <c r="I47" s="103">
         <f t="shared" si="7"/>
-        <v>-0.12286932581186043</v>
-      </c>
-      <c r="J46" s="104">
-        <v>0.3</v>
-      </c>
-      <c r="K46" s="103">
+        <v>-0.11898075207832921</v>
+      </c>
+      <c r="J47" s="104">
+        <v>0.35</v>
+      </c>
+      <c r="K47" s="103">
         <f t="shared" si="8"/>
-        <v>-4.0230867317060007E-2</v>
-      </c>
-      <c r="L46" s="104">
-        <v>0.87</v>
-      </c>
-      <c r="M46" s="105">
+        <v>-3.3186318329401797E-2</v>
+      </c>
+      <c r="L47" s="104">
+        <v>0.88</v>
+      </c>
+      <c r="M47" s="105">
         <f t="shared" si="9"/>
-        <v>8.4549328363533544E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="12">
+        <v>9.239283072182787E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="12">
         <v>45082</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C48" s="18">
         <v>155.820007</v>
       </c>
-      <c r="D47">
+      <c r="D48" s="126">
         <f t="shared" si="0"/>
         <v>-7.6949466757081364E-4</v>
       </c>
-      <c r="H47" s="102">
-        <v>0.04</v>
-      </c>
-      <c r="I47" s="103">
+      <c r="H48" s="102">
+        <v>0.05</v>
+      </c>
+      <c r="I48" s="103">
         <f t="shared" si="7"/>
-        <v>-0.11919323922707813</v>
-      </c>
-      <c r="J47" s="104">
-        <v>0.35</v>
-      </c>
-      <c r="K47" s="103">
+        <v>-0.11445520810419088</v>
+      </c>
+      <c r="J48" s="104">
+        <v>0.4</v>
+      </c>
+      <c r="K48" s="103">
         <f t="shared" si="8"/>
-        <v>-3.3296461362503096E-2</v>
-      </c>
-      <c r="L47" s="104">
-        <v>0.88</v>
-      </c>
-      <c r="M47" s="105">
+        <v>-2.5279682784335612E-2</v>
+      </c>
+      <c r="L48" s="104">
+        <v>0.89</v>
+      </c>
+      <c r="M48" s="105">
         <f t="shared" si="9"/>
-        <v>9.0340008570796215E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="12">
+        <v>9.7320570385347596E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="12">
         <v>45075</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C49" s="18">
         <v>155.94000199999999</v>
       </c>
-      <c r="D48">
+      <c r="D49" s="126">
         <f t="shared" si="0"/>
         <v>4.5594763615359746E-2</v>
       </c>
-      <c r="H48" s="102">
-        <v>0.05</v>
-      </c>
-      <c r="I48" s="103">
+      <c r="H49" s="102">
+        <v>0.06</v>
+      </c>
+      <c r="I49" s="103">
         <f t="shared" si="7"/>
-        <v>-0.11468631143353698</v>
-      </c>
-      <c r="J48" s="104">
-        <v>0.4</v>
-      </c>
-      <c r="K48" s="103">
+        <v>-0.10879651845152354</v>
+      </c>
+      <c r="J49" s="104">
+        <v>0.45</v>
+      </c>
+      <c r="K49" s="103">
         <f t="shared" si="8"/>
-        <v>-2.5335766555049453E-2</v>
-      </c>
-      <c r="L48" s="104">
-        <v>0.89</v>
-      </c>
-      <c r="M48" s="105">
+        <v>-9.9837971567683058E-3</v>
+      </c>
+      <c r="L49" s="104">
+        <v>0.9</v>
+      </c>
+      <c r="M49" s="105">
         <f t="shared" si="9"/>
-        <v>9.4078735465797259E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="12">
+        <v>0.10078017418895337</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="12">
         <v>45068</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C50" s="18">
         <v>149.13999899999999</v>
       </c>
-      <c r="D49">
+      <c r="D50" s="126">
         <f t="shared" si="0"/>
         <v>-8.0479344975883382E-3</v>
       </c>
-      <c r="H49" s="102">
-        <v>0.06</v>
-      </c>
-      <c r="I49" s="103">
+      <c r="H50" s="102">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I50" s="103">
         <f t="shared" si="7"/>
-        <v>-0.10896946034280479</v>
-      </c>
-      <c r="J49" s="104">
-        <v>0.45</v>
-      </c>
-      <c r="K49" s="103">
+        <v>-0.10204440895798403</v>
+      </c>
+      <c r="J50" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="K50" s="103">
         <f t="shared" si="8"/>
-        <v>-1.0689776138282188E-2</v>
-      </c>
-      <c r="L49" s="104">
-        <v>0.9</v>
-      </c>
-      <c r="M49" s="105">
+        <v>-7.6949466757081364E-4</v>
+      </c>
+      <c r="L50" s="104">
+        <v>0.91</v>
+      </c>
+      <c r="M50" s="105">
         <f t="shared" si="9"/>
-        <v>9.9488472841472525E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="12">
+        <v>0.10317625024150698</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="12">
         <v>45061</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C51" s="18">
         <v>150.35000600000001</v>
       </c>
-      <c r="D50">
+      <c r="D51" s="126">
         <f t="shared" si="0"/>
         <v>6.2919824593562934E-2</v>
       </c>
-      <c r="H50" s="102">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I50" s="103">
+      <c r="H51" s="102">
+        <v>0.08</v>
+      </c>
+      <c r="I51" s="103">
         <f t="shared" si="7"/>
-        <v>-0.10244419641056943</v>
-      </c>
-      <c r="J50" s="104">
-        <v>0.5</v>
-      </c>
-      <c r="K50" s="103">
+        <v>-9.9512745258046473E-2</v>
+      </c>
+      <c r="J51" s="104">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K51" s="103">
         <f t="shared" si="8"/>
-        <v>-1.5901968203113626E-3</v>
-      </c>
-      <c r="L50" s="104">
-        <v>0.91</v>
-      </c>
-      <c r="M50" s="105">
+        <v>9.8449578755132553E-3</v>
+      </c>
+      <c r="L51" s="104">
+        <v>0.92</v>
+      </c>
+      <c r="M51" s="105">
         <f t="shared" si="9"/>
-        <v>0.10147642181528681</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="12">
+        <v>0.10821056944203931</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="12">
         <v>45054</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C52" s="18">
         <v>141.449997</v>
       </c>
-      <c r="D51">
+      <c r="D52" s="126">
         <f t="shared" si="0"/>
         <v>0.14478795151809565</v>
       </c>
-      <c r="H51" s="102">
-        <v>0.08</v>
-      </c>
-      <c r="I51" s="103">
+      <c r="H52" s="102">
+        <v>0.09</v>
+      </c>
+      <c r="I52" s="103">
         <f t="shared" si="7"/>
-        <v>-9.9650422271656464E-2</v>
-      </c>
-      <c r="J51" s="104">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K51" s="103">
+        <v>-9.7390301868346102E-2</v>
+      </c>
+      <c r="J52" s="104">
+        <v>0.6</v>
+      </c>
+      <c r="K52" s="103">
         <f t="shared" si="8"/>
-        <v>9.1473876828580929E-3</v>
-      </c>
-      <c r="L51" s="104">
-        <v>0.92</v>
-      </c>
-      <c r="M51" s="105">
+        <v>1.7254033487822357E-2</v>
+      </c>
+      <c r="L52" s="104">
+        <v>0.93</v>
+      </c>
+      <c r="M52" s="105">
         <f t="shared" si="9"/>
-        <v>0.10462374611731237</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="12">
+        <v>0.11170240197046544</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="12">
         <v>45047</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C53" s="18">
         <v>123.55999799999999</v>
       </c>
-      <c r="D52">
+      <c r="D53" s="126">
         <f t="shared" si="0"/>
         <v>-9.253823171156772E-2</v>
       </c>
-      <c r="H52" s="102">
-        <v>0.09</v>
-      </c>
-      <c r="I52" s="103">
+      <c r="H53" s="102">
+        <v>0.1</v>
+      </c>
+      <c r="I53" s="103">
         <f t="shared" si="7"/>
-        <v>-9.7508112708440786E-2</v>
-      </c>
-      <c r="J52" s="104">
-        <v>0.6</v>
-      </c>
-      <c r="K52" s="103">
+        <v>-9.6379519752041148E-2</v>
+      </c>
+      <c r="J53" s="104">
+        <v>0.65</v>
+      </c>
+      <c r="K53" s="103">
         <f t="shared" si="8"/>
-        <v>1.5843210028717657E-2</v>
-      </c>
-      <c r="L52" s="104">
-        <v>0.93</v>
-      </c>
-      <c r="M52" s="105">
+        <v>3.0877489353101004E-2</v>
+      </c>
+      <c r="L53" s="104">
+        <v>0.94</v>
+      </c>
+      <c r="M53" s="105">
         <f t="shared" si="9"/>
-        <v>0.11027416494956492</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="12">
+        <v>0.11831121482599063</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="12">
         <v>45040</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C54" s="18">
         <v>136.16000399999999</v>
       </c>
-      <c r="D53">
+      <c r="D54" s="126">
         <f t="shared" si="0"/>
         <v>-3.3091910015314974E-2</v>
       </c>
-      <c r="H53" s="102">
-        <v>0.1</v>
-      </c>
-      <c r="I53" s="103">
+      <c r="H54" s="102">
+        <v>0.11</v>
+      </c>
+      <c r="I54" s="103">
         <f t="shared" si="7"/>
-        <v>-9.673305032079009E-2</v>
-      </c>
-      <c r="J53" s="104">
-        <v>0.65</v>
-      </c>
-      <c r="K53" s="103">
+        <v>-9.2923188237950857E-2</v>
+      </c>
+      <c r="J54" s="104">
+        <v>0.7</v>
+      </c>
+      <c r="K54" s="103">
         <f t="shared" si="8"/>
-        <v>2.9327136499677098E-2</v>
-      </c>
-      <c r="L53" s="104">
-        <v>0.94</v>
-      </c>
-      <c r="M53" s="105">
+        <v>4.5303098061554296E-2</v>
+      </c>
+      <c r="L54" s="104">
+        <v>0.95</v>
+      </c>
+      <c r="M54" s="105">
         <f t="shared" si="9"/>
-        <v>0.11889593002999232</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="12">
+        <v>0.13616683810220143</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="12">
         <v>45033</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C55" s="18">
         <v>140.820007</v>
       </c>
-      <c r="D54">
+      <c r="D55" s="126">
         <f t="shared" si="0"/>
         <v>4.3884457103830599E-2</v>
       </c>
-      <c r="H54" s="102">
-        <v>0.11</v>
-      </c>
-      <c r="I54" s="103">
+      <c r="H55" s="102">
+        <v>0.12</v>
+      </c>
+      <c r="I55" s="103">
         <f t="shared" si="7"/>
-        <v>-9.3034623021903864E-2</v>
-      </c>
-      <c r="J54" s="104">
-        <v>0.7</v>
-      </c>
-      <c r="K54" s="103">
+        <v>-8.9827051971558824E-2</v>
+      </c>
+      <c r="J55" s="104">
+        <v>0.75</v>
+      </c>
+      <c r="K55" s="103">
         <f t="shared" si="8"/>
-        <v>4.4937719224913401E-2</v>
-      </c>
-      <c r="L54" s="104">
-        <v>0.95</v>
-      </c>
-      <c r="M54" s="105">
+        <v>6.2914696961257399E-2</v>
+      </c>
+      <c r="L55" s="104">
+        <v>0.96</v>
+      </c>
+      <c r="M55" s="105">
         <f t="shared" si="9"/>
-        <v>0.1368772876304343</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="12">
+        <v>0.14843756857005316</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" s="12">
         <v>45026</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C56" s="18">
         <v>134.89999399999999</v>
       </c>
-      <c r="D55">
+      <c r="D56" s="126">
         <f t="shared" si="0"/>
         <v>-1.3384056560639457E-2</v>
       </c>
-      <c r="H55" s="102">
-        <v>0.12</v>
-      </c>
-      <c r="I55" s="103">
+      <c r="H56" s="102">
+        <v>0.13</v>
+      </c>
+      <c r="I56" s="103">
         <f t="shared" si="7"/>
-        <v>-9.0285974142513506E-2</v>
-      </c>
-      <c r="J55" s="104">
-        <v>0.75</v>
-      </c>
-      <c r="K55" s="103">
+        <v>-8.3227107193970001E-2</v>
+      </c>
+      <c r="J56" s="104">
+        <v>0.8</v>
+      </c>
+      <c r="K56" s="103">
         <f t="shared" si="8"/>
-        <v>6.0146669574573652E-2</v>
-      </c>
-      <c r="L55" s="104">
-        <v>0.96</v>
-      </c>
-      <c r="M55" s="105">
+        <v>7.1660573956005891E-2</v>
+      </c>
+      <c r="L56" s="104">
+        <v>0.97</v>
+      </c>
+      <c r="M56" s="105">
         <f t="shared" si="9"/>
-        <v>0.14889377070154777</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="12">
+        <v>0.15761206168287051</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="12">
         <v>45019</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C57" s="18">
         <v>136.729996</v>
       </c>
-      <c r="D56">
+      <c r="D57" s="126">
         <f t="shared" si="0"/>
         <v>-4.1096852264446482E-2</v>
       </c>
-      <c r="H56" s="102">
-        <v>0.13</v>
-      </c>
-      <c r="I56" s="103">
-        <f t="shared" si="7"/>
-        <v>-8.3307983104005945E-2</v>
-      </c>
-      <c r="J56" s="104">
-        <v>0.8</v>
-      </c>
-      <c r="K56" s="103">
-        <f t="shared" si="8"/>
-        <v>7.0619138745168716E-2</v>
-      </c>
-      <c r="L56" s="104">
-        <v>0.97</v>
-      </c>
-      <c r="M56" s="105">
-        <f t="shared" si="9"/>
-        <v>0.15766959101573838</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="12">
-        <v>45012</v>
-      </c>
-      <c r="C57" s="18">
-        <v>142.58999600000001</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="0"/>
-        <v>4.4538870578670897E-2</v>
-      </c>
       <c r="H57" s="102">
         <v>0.14000000000000001</v>
       </c>
       <c r="I57" s="103">
         <f t="shared" si="7"/>
-        <v>-8.2319553233469747E-2</v>
+        <v>-8.2211411203507292E-2</v>
       </c>
       <c r="J57" s="104"/>
       <c r="K57" s="103"/>
@@ -26930,26 +26929,26 @@
       </c>
       <c r="M57" s="105">
         <f t="shared" si="9"/>
-        <v>0.32897174879189922</v>
+        <v>0.32882176490781712</v>
       </c>
     </row>
     <row r="58" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="12">
-        <v>45005</v>
+        <v>45012</v>
       </c>
       <c r="C58" s="18">
-        <v>136.509995</v>
-      </c>
-      <c r="D58">
+        <v>142.58999600000001</v>
+      </c>
+      <c r="D58" s="126">
         <f t="shared" si="0"/>
-        <v>8.0668104813172992E-2</v>
+        <v>4.4538870578670897E-2</v>
       </c>
       <c r="H58" s="106">
         <v>0.15</v>
       </c>
       <c r="I58" s="107">
         <f t="shared" si="7"/>
-        <v>-7.9947727627092097E-2</v>
+        <v>-7.9609930189779188E-2</v>
       </c>
       <c r="J58" s="108"/>
       <c r="K58" s="87"/>
@@ -26958,92 +26957,92 @@
       </c>
       <c r="M58" s="110">
         <f t="shared" si="9"/>
-        <v>0.34844377950232808</v>
+        <v>0.34821797117244579</v>
       </c>
     </row>
     <row r="59" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="12">
+        <v>45005</v>
+      </c>
+      <c r="C59" s="18">
+        <v>136.509995</v>
+      </c>
+      <c r="D59" s="126">
+        <f t="shared" si="0"/>
+        <v>8.0668104813172992E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60" s="12">
         <v>44998</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C60" s="18">
         <v>126.32</v>
       </c>
-      <c r="D59">
+      <c r="D60" s="126">
         <f t="shared" si="0"/>
         <v>7.2508074991578075E-2</v>
       </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="12">
+      <c r="H60" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="I60" s="112"/>
+    </row>
+    <row r="61" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="12">
         <v>44991</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C61" s="18">
         <v>117.779999</v>
       </c>
-      <c r="D60">
+      <c r="D61" s="126">
         <f t="shared" si="0"/>
         <v>-1.2492647249752187E-2</v>
       </c>
-      <c r="H60" s="111" t="s">
-        <v>127</v>
-      </c>
-      <c r="I60" s="112"/>
-    </row>
-    <row r="61" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="12">
+      <c r="H61" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="I61" s="114"/>
+    </row>
+    <row r="62" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="12">
         <v>44984</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C62" s="18">
         <v>119.269997</v>
       </c>
-      <c r="D61">
+      <c r="D62" s="126">
         <f t="shared" si="0"/>
         <v>0.36840283990808453</v>
       </c>
-      <c r="H61" s="113" t="s">
-        <v>128</v>
-      </c>
-      <c r="I61" s="114"/>
-    </row>
-    <row r="62" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="12">
+      <c r="H62" s="115"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="12">
         <v>44977</v>
       </c>
-      <c r="C62" s="18">
+      <c r="C63" s="18">
         <v>87.160004000000001</v>
       </c>
-      <c r="D62">
+      <c r="D63" s="126">
         <f t="shared" si="0"/>
         <v>-4.5762997405868089E-2</v>
       </c>
-      <c r="H62" s="115"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="12">
+      <c r="H63" s="111" t="s">
+        <v>129</v>
+      </c>
+      <c r="I63" s="116"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64" s="12">
         <v>44970</v>
       </c>
-      <c r="C63" s="18">
+      <c r="C64" s="18">
         <v>91.339995999999999</v>
       </c>
-      <c r="D63">
+      <c r="D64" s="126">
         <f t="shared" si="0"/>
         <v>-2.9473310452207135E-3</v>
-      </c>
-      <c r="H63" s="111" t="s">
-        <v>129</v>
-      </c>
-      <c r="I63" s="116"/>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="12">
-        <v>44963</v>
-      </c>
-      <c r="C64" s="18">
-        <v>91.610000999999997</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="0"/>
-        <v>-8.2891161106128375E-2</v>
       </c>
       <c r="H64" s="117" t="s">
         <v>130</v>
@@ -27055,14 +27054,14 @@
     </row>
     <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="12">
-        <v>44956</v>
+        <v>44963</v>
       </c>
       <c r="C65" s="18">
-        <v>99.889999000000003</v>
-      </c>
-      <c r="D65">
+        <v>91.610000999999997</v>
+      </c>
+      <c r="D65" s="126">
         <f t="shared" si="0"/>
-        <v>7.3739654667737797E-2</v>
+        <v>-8.2891161106128375E-2</v>
       </c>
       <c r="H65" s="113" t="s">
         <v>131</v>
@@ -27074,945 +27073,957 @@
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="12">
-        <v>44949</v>
+        <v>44956</v>
       </c>
       <c r="C66" s="18">
-        <v>93.029999000000004</v>
-      </c>
-      <c r="D66">
+        <v>99.889999000000003</v>
+      </c>
+      <c r="D66" s="126">
         <f t="shared" si="0"/>
-        <v>9.9905377159958064E-2</v>
+        <v>7.3739654667737797E-2</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="12">
-        <v>44942</v>
+        <v>44949</v>
       </c>
       <c r="C67" s="18">
-        <v>84.580001999999993</v>
-      </c>
-      <c r="D67">
+        <v>93.029999000000004</v>
+      </c>
+      <c r="D67" s="126">
         <f t="shared" ref="D67:D130" si="10">C67/C68-1</f>
-        <v>6.5776221449392436E-2</v>
+        <v>9.9905377159958064E-2</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="12">
+        <v>44942</v>
+      </c>
+      <c r="C68" s="18">
+        <v>84.580001999999993</v>
+      </c>
+      <c r="D68" s="126">
+        <f t="shared" si="10"/>
+        <v>6.5776221449392436E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="12">
         <v>44935</v>
       </c>
-      <c r="C68" s="18">
+      <c r="C69" s="18">
         <v>79.360000999999997</v>
       </c>
-      <c r="D68">
+      <c r="D69" s="126">
         <f t="shared" si="10"/>
         <v>0.10099887344620218</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="12">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="12">
         <v>44928</v>
       </c>
-      <c r="C69" s="18">
+      <c r="C70" s="18">
         <v>72.080001999999993</v>
       </c>
-      <c r="D69">
+      <c r="D70" s="126">
         <f t="shared" si="10"/>
         <v>1.3355898215488438E-2</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="12">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="12">
         <v>44921</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C71" s="18">
         <v>71.129997000000003</v>
       </c>
-      <c r="D70">
+      <c r="D71" s="126">
         <f t="shared" si="10"/>
         <v>6.0820370331842177E-3</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="12">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="12">
         <v>44914</v>
       </c>
-      <c r="C71" s="18">
+      <c r="C72" s="18">
         <v>70.699996999999996</v>
       </c>
-      <c r="D71">
+      <c r="D72" s="126">
         <f t="shared" si="10"/>
         <v>-3.1374175404142446E-2</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="12">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="12">
         <v>44907</v>
       </c>
-      <c r="C72" s="18">
+      <c r="C73" s="18">
         <v>72.989998</v>
       </c>
-      <c r="D72">
+      <c r="D73" s="126">
         <f t="shared" si="10"/>
         <v>6.2909569328951864E-2</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="12">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="12">
         <v>44900</v>
       </c>
-      <c r="C73" s="18">
+      <c r="C74" s="18">
         <v>68.669998000000007</v>
       </c>
-      <c r="D73">
+      <c r="D74" s="126">
         <f t="shared" si="10"/>
         <v>-2.8712858361224392E-2</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="12">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="12">
         <v>44893</v>
       </c>
-      <c r="C74" s="18">
+      <c r="C75" s="18">
         <v>70.699996999999996</v>
       </c>
-      <c r="D74">
+      <c r="D75" s="126">
         <f t="shared" si="10"/>
         <v>1.4492681460964718E-2</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="12">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="12">
         <v>44886</v>
       </c>
-      <c r="C75" s="18">
+      <c r="C76" s="18">
         <v>69.690002000000007</v>
       </c>
-      <c r="D75">
+      <c r="D76" s="126">
         <f t="shared" si="10"/>
         <v>2.9394462159282098E-2</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="12">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="12">
         <v>44879</v>
       </c>
-      <c r="C76" s="18">
+      <c r="C77" s="18">
         <v>67.699996999999996</v>
       </c>
-      <c r="D76">
+      <c r="D77" s="126">
         <f t="shared" si="10"/>
         <v>-7.8033542148985613E-2</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="12">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="12">
         <v>44872</v>
       </c>
-      <c r="C77" s="18">
+      <c r="C78" s="18">
         <v>73.430000000000007</v>
       </c>
-      <c r="D77">
+      <c r="D78" s="126">
         <f t="shared" si="10"/>
         <v>-8.0285525064405006E-2</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="12">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="12">
         <v>44865</v>
       </c>
-      <c r="C78" s="18">
+      <c r="C79" s="18">
         <v>79.839995999999999</v>
       </c>
-      <c r="D78">
+      <c r="D79" s="126">
         <f t="shared" si="10"/>
         <v>-3.9807647869930296E-2</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="12">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="12">
         <v>44858</v>
       </c>
-      <c r="C79" s="18">
+      <c r="C80" s="18">
         <v>83.150002000000001</v>
       </c>
-      <c r="D79">
+      <c r="D80" s="126">
         <f t="shared" si="10"/>
         <v>1.0942273556231008E-2</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="12">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="12">
         <v>44851</v>
       </c>
-      <c r="C80" s="18">
+      <c r="C81" s="18">
         <v>82.25</v>
       </c>
-      <c r="D80">
+      <c r="D81" s="126">
         <f t="shared" si="10"/>
         <v>5.0312885974023391E-2</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="12">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="12">
         <v>44844</v>
       </c>
-      <c r="C81" s="18">
+      <c r="C82" s="18">
         <v>78.309997999999993</v>
       </c>
-      <c r="D81">
+      <c r="D82" s="126">
         <f t="shared" si="10"/>
         <v>-0.20497463959390871</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="12">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="12">
         <v>44837</v>
       </c>
-      <c r="C82" s="18">
+      <c r="C83" s="18">
         <v>98.5</v>
       </c>
-      <c r="D82">
+      <c r="D83" s="126">
         <f t="shared" si="10"/>
         <v>3.4337886138678497E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="12">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="12">
         <v>44830</v>
       </c>
-      <c r="C83" s="18">
+      <c r="C84" s="18">
         <v>95.230002999999996</v>
       </c>
-      <c r="D83">
+      <c r="D84" s="126">
         <f t="shared" si="10"/>
         <v>6.7481269672472477E-2</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="12">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="12">
         <v>44823</v>
       </c>
-      <c r="C84" s="18">
+      <c r="C85" s="18">
         <v>89.209998999999996</v>
       </c>
-      <c r="D84">
+      <c r="D85" s="126">
         <f t="shared" si="10"/>
         <v>-0.10170173399862514</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="12">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="12">
         <v>44816</v>
       </c>
-      <c r="C85" s="18">
+      <c r="C86" s="18">
         <v>99.309997999999993</v>
       </c>
-      <c r="D85">
+      <c r="D86" s="126">
         <f t="shared" si="10"/>
         <v>-2.4108989730519115E-3</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="12">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="12">
         <v>44809</v>
       </c>
-      <c r="C86" s="18">
+      <c r="C87" s="18">
         <v>99.550003000000004</v>
       </c>
-      <c r="D86">
+      <c r="D87" s="126">
         <f t="shared" si="10"/>
         <v>7.2274960029080626E-2</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="12">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="12">
         <v>44802</v>
       </c>
-      <c r="C87" s="18">
+      <c r="C88" s="18">
         <v>92.839995999999999</v>
       </c>
-      <c r="D87">
+      <c r="D88" s="126">
         <f t="shared" si="10"/>
         <v>-4.6102821253442006E-3</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="12">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="12">
         <v>44795</v>
       </c>
-      <c r="C88" s="18">
+      <c r="C89" s="18">
         <v>93.269997000000004</v>
       </c>
-      <c r="D88">
+      <c r="D89" s="126">
         <f t="shared" si="10"/>
         <v>-2.5391850325763299E-2</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="12">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="12">
         <v>44788</v>
       </c>
-      <c r="C89" s="18">
+      <c r="C90" s="18">
         <v>95.699996999999996</v>
       </c>
-      <c r="D89">
+      <c r="D90" s="126">
         <f t="shared" si="10"/>
         <v>-0.11728085488833784</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="12">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="12">
         <v>44781</v>
       </c>
-      <c r="C90" s="18">
+      <c r="C91" s="18">
         <v>108.415001</v>
       </c>
-      <c r="D90">
+      <c r="D91" s="126">
         <f t="shared" si="10"/>
         <v>5.1857970311439017E-2</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="12">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="12">
         <v>44774</v>
       </c>
-      <c r="C91" s="18">
+      <c r="C92" s="18">
         <v>103.07</v>
       </c>
-      <c r="D91">
+      <c r="D92" s="126">
         <f t="shared" si="10"/>
         <v>0.12337874659400527</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="12">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="12">
         <v>44767</v>
       </c>
-      <c r="C92" s="18">
+      <c r="C93" s="18">
         <v>91.75</v>
       </c>
-      <c r="D92">
+      <c r="D93" s="126">
         <f t="shared" si="10"/>
         <v>-3.8763720443071303E-2</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="12">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="12">
         <v>44760</v>
       </c>
-      <c r="C93" s="18">
+      <c r="C94" s="18">
         <v>95.449996999999996</v>
       </c>
-      <c r="D93">
+      <c r="D94" s="126">
         <f t="shared" si="10"/>
         <v>-3.9738480085744876E-2</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="12">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="12">
         <v>44753</v>
       </c>
-      <c r="C94" s="18">
+      <c r="C95" s="18">
         <v>99.400002000000001</v>
       </c>
-      <c r="D94">
+      <c r="D95" s="126">
         <f t="shared" si="10"/>
         <v>-9.7102319814781346E-2</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="12">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="12">
         <v>44746</v>
       </c>
-      <c r="C95" s="18">
+      <c r="C96" s="18">
         <v>110.089996</v>
       </c>
-      <c r="D95">
+      <c r="D96" s="126">
         <f t="shared" si="10"/>
         <v>0.158110649234392</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="12">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="12">
         <v>44739</v>
       </c>
-      <c r="C96" s="18">
+      <c r="C97" s="18">
         <v>95.059997999999993</v>
       </c>
-      <c r="D96">
+      <c r="D97" s="126">
         <f t="shared" si="10"/>
         <v>-6.5565760378479498E-2</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="12">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="12">
         <v>44732</v>
       </c>
-      <c r="C97" s="18">
+      <c r="C98" s="18">
         <v>101.730003</v>
       </c>
-      <c r="D97">
+      <c r="D98" s="126">
         <f t="shared" si="10"/>
         <v>7.4121043967068312E-2</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="12">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="12">
         <v>44725</v>
       </c>
-      <c r="C98" s="18">
+      <c r="C99" s="18">
         <v>94.709998999999996</v>
       </c>
-      <c r="D98">
+      <c r="D99" s="126">
         <f t="shared" si="10"/>
         <v>1.4351461464556126E-2</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="12">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="12">
         <v>44718</v>
       </c>
-      <c r="C99" s="18">
+      <c r="C100" s="18">
         <v>93.370002999999997</v>
       </c>
-      <c r="D99">
+      <c r="D100" s="126">
         <f t="shared" si="10"/>
         <v>4.5108654359017342E-2</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="12">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="12">
         <v>44711</v>
       </c>
-      <c r="C100" s="18">
+      <c r="C101" s="18">
         <v>89.339995999999999</v>
       </c>
-      <c r="D100">
+      <c r="D101" s="126">
         <f t="shared" si="10"/>
         <v>6.63642524034882E-2</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="12">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="12">
         <v>44704</v>
       </c>
-      <c r="C101" s="18">
+      <c r="C102" s="18">
         <v>83.779999000000004</v>
       </c>
-      <c r="D101">
+      <c r="D102" s="126">
         <f t="shared" si="10"/>
         <v>9.5736333975102506E-2</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="12">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="12">
         <v>44697</v>
       </c>
-      <c r="C102" s="18">
+      <c r="C103" s="18">
         <v>76.459998999999996</v>
       </c>
-      <c r="D102">
+      <c r="D103" s="126">
         <f t="shared" si="10"/>
         <v>-0.148267778153095</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="12">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="12">
         <v>44690</v>
       </c>
-      <c r="C103" s="18">
+      <c r="C104" s="18">
         <v>89.769997000000004</v>
       </c>
-      <c r="D103">
+      <c r="D104" s="126">
         <f t="shared" si="10"/>
         <v>0.11363349319397731</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="12">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="12">
         <v>44683</v>
       </c>
-      <c r="C104" s="18">
+      <c r="C105" s="18">
         <v>80.610000999999997</v>
       </c>
-      <c r="D104">
+      <c r="D105" s="126">
         <f t="shared" si="10"/>
         <v>-6.7769167714014533E-2</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="12">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="12">
         <v>44676</v>
       </c>
-      <c r="C105" s="18">
+      <c r="C106" s="18">
         <v>86.470000999999996</v>
       </c>
-      <c r="D105">
+      <c r="D106" s="126">
         <f t="shared" si="10"/>
         <v>5.465127906976619E-3</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="12">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="12">
         <v>44669</v>
       </c>
-      <c r="C106" s="18">
+      <c r="C107" s="18">
         <v>86</v>
       </c>
-      <c r="D106">
+      <c r="D107" s="126">
         <f t="shared" si="10"/>
         <v>-4.2529503451347095E-2</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="12">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="12">
         <v>44662</v>
       </c>
-      <c r="C107" s="18">
+      <c r="C108" s="18">
         <v>89.82</v>
       </c>
-      <c r="D107">
+      <c r="D108" s="126">
         <f t="shared" si="10"/>
         <v>-5.0126883462920602E-2</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="12">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="12">
         <v>44655</v>
       </c>
-      <c r="C108" s="18">
+      <c r="C109" s="18">
         <v>94.559997999999993</v>
       </c>
-      <c r="D108">
+      <c r="D109" s="126">
         <f t="shared" si="10"/>
         <v>-1.1395755119796069E-2</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="12">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="12">
         <v>44648</v>
       </c>
-      <c r="C109" s="18">
+      <c r="C110" s="18">
         <v>95.650002000000001</v>
       </c>
-      <c r="D109">
+      <c r="D110" s="126">
         <f t="shared" si="10"/>
         <v>2.7941955036798749E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="12">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="12">
         <v>44641</v>
       </c>
-      <c r="C110" s="18">
+      <c r="C111" s="18">
         <v>93.050003000000004</v>
       </c>
-      <c r="D110">
+      <c r="D111" s="126">
         <f t="shared" si="10"/>
         <v>4.9278337843933206E-2</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="12">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="12">
         <v>44634</v>
       </c>
-      <c r="C111" s="18">
+      <c r="C112" s="18">
         <v>88.68</v>
       </c>
-      <c r="D111">
+      <c r="D112" s="126">
         <f t="shared" si="10"/>
         <v>0.15619300480546316</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="12">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="12">
         <v>44627</v>
       </c>
-      <c r="C112" s="18">
+      <c r="C113" s="18">
         <v>76.699996999999996</v>
       </c>
-      <c r="D112">
+      <c r="D113" s="126">
         <f t="shared" si="10"/>
         <v>2.7048701124799068E-2</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="12">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="12">
         <v>44620</v>
       </c>
-      <c r="C113" s="18">
+      <c r="C114" s="18">
         <v>74.680000000000007</v>
       </c>
-      <c r="D113">
+      <c r="D114" s="126">
         <f t="shared" si="10"/>
         <v>-0.15097770749178829</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="12">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="12">
         <v>44613</v>
       </c>
-      <c r="C114" s="18">
+      <c r="C115" s="18">
         <v>87.959998999999996</v>
       </c>
-      <c r="D114">
+      <c r="D115" s="126">
         <f t="shared" si="10"/>
         <v>-3.3406604395604389E-2</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="12">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="12">
         <v>44606</v>
       </c>
-      <c r="C115" s="18">
+      <c r="C116" s="18">
         <v>91</v>
       </c>
-      <c r="D115">
+      <c r="D116" s="126">
         <f t="shared" si="10"/>
         <v>-3.1914893617021267E-2</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="12">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="12">
         <v>44599</v>
       </c>
-      <c r="C116" s="18">
+      <c r="C117" s="18">
         <v>94</v>
       </c>
-      <c r="D116">
+      <c r="D117" s="126">
         <f t="shared" si="10"/>
         <v>2.7546971112364371E-2</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="12">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="12">
         <v>44592</v>
       </c>
-      <c r="C117" s="18">
+      <c r="C118" s="18">
         <v>91.480002999999996</v>
       </c>
-      <c r="D117">
+      <c r="D118" s="126">
         <f t="shared" si="10"/>
         <v>-3.8113796403924649E-3</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="12">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="12">
         <v>44585</v>
       </c>
-      <c r="C118" s="18">
+      <c r="C119" s="18">
         <v>91.830001999999993</v>
       </c>
-      <c r="D118">
+      <c r="D119" s="126">
         <f t="shared" si="10"/>
         <v>7.1403606013342724E-2</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="12">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="12">
         <v>44578</v>
       </c>
-      <c r="C119" s="18">
+      <c r="C120" s="18">
         <v>85.709998999999996</v>
       </c>
-      <c r="D119">
+      <c r="D120" s="126">
         <f t="shared" si="10"/>
         <v>-7.4705799677398321E-2</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="12">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="12">
         <v>44571</v>
       </c>
-      <c r="C120" s="18">
+      <c r="C121" s="18">
         <v>92.629997000000003</v>
       </c>
-      <c r="D120">
+      <c r="D121" s="126">
         <f t="shared" si="10"/>
         <v>-9.3551275202049644E-2</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="12">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="12">
         <v>44564</v>
       </c>
-      <c r="C121" s="18">
+      <c r="C122" s="18">
         <v>102.19000200000001</v>
       </c>
-      <c r="D121">
+      <c r="D122" s="126">
         <f t="shared" si="10"/>
         <v>-3.6942785440177262E-2</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="12">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="12">
         <v>44557</v>
       </c>
-      <c r="C122" s="18">
+      <c r="C123" s="18">
         <v>106.110001</v>
       </c>
-      <c r="D122">
+      <c r="D123" s="126">
         <f t="shared" si="10"/>
         <v>-2.6156369549893199E-2</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="12">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="12">
         <v>44550</v>
       </c>
-      <c r="C123" s="18">
+      <c r="C124" s="18">
         <v>108.959999</v>
       </c>
-      <c r="D123">
+      <c r="D124" s="126">
         <f t="shared" si="10"/>
         <v>4.228044727108804E-2</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="12">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="12">
         <v>44543</v>
       </c>
-      <c r="C124" s="18">
+      <c r="C125" s="18">
         <v>104.540001</v>
       </c>
-      <c r="D124">
+      <c r="D125" s="126">
         <f t="shared" si="10"/>
         <v>9.2486140819602047E-2</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="12">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="12">
         <v>44536</v>
       </c>
-      <c r="C125" s="18">
+      <c r="C126" s="18">
         <v>95.690002000000007</v>
       </c>
-      <c r="D125">
+      <c r="D126" s="126">
         <f t="shared" si="10"/>
         <v>-0.12259303360706086</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="12">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="12">
         <v>44529</v>
       </c>
-      <c r="C126" s="18">
+      <c r="C127" s="18">
         <v>109.05999799999999</v>
       </c>
-      <c r="D126">
+      <c r="D127" s="126">
         <f t="shared" si="10"/>
         <v>-0.11029534817596109</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="12">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="12">
         <v>44522</v>
       </c>
-      <c r="C127" s="18">
+      <c r="C128" s="18">
         <v>122.58000199999999</v>
       </c>
-      <c r="D127">
+      <c r="D128" s="126">
         <f t="shared" si="10"/>
         <v>-9.8411329149166615E-2</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="12">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="12">
         <v>44515</v>
       </c>
-      <c r="C128" s="18">
+      <c r="C129" s="18">
         <v>135.96000699999999</v>
       </c>
-      <c r="D128">
+      <c r="D129" s="126">
         <f t="shared" si="10"/>
         <v>-0.12295185465225511</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="12">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="12">
         <v>44508</v>
       </c>
-      <c r="C129" s="18">
+      <c r="C130" s="18">
         <v>155.020004</v>
       </c>
-      <c r="D129">
+      <c r="D130" s="126">
         <f t="shared" si="10"/>
         <v>8.3913877159016437E-3</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="12">
-        <v>44501</v>
-      </c>
-      <c r="C130" s="18">
-        <v>153.729996</v>
-      </c>
-      <c r="D130">
-        <f t="shared" si="10"/>
-        <v>-0.11491741476288309</v>
-      </c>
-    </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="12">
-        <v>44494</v>
+        <v>44501</v>
       </c>
       <c r="C131" s="18">
-        <v>173.69000199999999</v>
-      </c>
-      <c r="D131">
-        <f t="shared" ref="D131:D143" si="11">C131/C132-1</f>
-        <v>-2.5636671873574435E-2</v>
+        <v>153.729996</v>
+      </c>
+      <c r="D131" s="126">
+        <f t="shared" ref="D131:D144" si="11">C131/C132-1</f>
+        <v>-0.11491741476288309</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="12">
+        <v>44494</v>
+      </c>
+      <c r="C132" s="18">
+        <v>173.69000199999999</v>
+      </c>
+      <c r="D132" s="126">
+        <f t="shared" si="11"/>
+        <v>-2.5636671873574435E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="12">
         <v>44487</v>
       </c>
-      <c r="C132" s="18">
+      <c r="C133" s="18">
         <v>178.259995</v>
       </c>
-      <c r="D132">
+      <c r="D133" s="126">
         <f t="shared" si="11"/>
         <v>0.13758773715866757</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="12">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="12">
         <v>44480</v>
       </c>
-      <c r="C133" s="18">
+      <c r="C134" s="18">
         <v>156.699997</v>
       </c>
-      <c r="D133">
+      <c r="D134" s="126">
         <f t="shared" si="11"/>
         <v>-5.8971935888255222E-2</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="12">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="12">
         <v>44473</v>
       </c>
-      <c r="C134" s="18">
+      <c r="C135" s="18">
         <v>166.520004</v>
       </c>
-      <c r="D134">
+      <c r="D135" s="126">
         <f t="shared" si="11"/>
         <v>3.6990919952784695E-2</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="12">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="12">
         <v>44466</v>
       </c>
-      <c r="C135" s="18">
+      <c r="C136" s="18">
         <v>160.58000200000001</v>
       </c>
-      <c r="D135">
+      <c r="D136" s="126">
         <f t="shared" si="11"/>
         <v>-0.19456284281895064</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="12">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="12">
         <v>44459</v>
       </c>
-      <c r="C136" s="18">
+      <c r="C137" s="18">
         <v>199.36999499999999</v>
       </c>
-      <c r="D136">
+      <c r="D137" s="126">
         <f t="shared" si="11"/>
         <v>7.7792190026860997E-2</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="12">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="12">
         <v>44452</v>
       </c>
-      <c r="C137" s="18">
+      <c r="C138" s="18">
         <v>184.979996</v>
       </c>
-      <c r="D137">
+      <c r="D138" s="126">
         <f t="shared" si="11"/>
         <v>6.6966610917881253E-2</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="12">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="12">
         <v>44445</v>
       </c>
-      <c r="C138" s="18">
+      <c r="C139" s="18">
         <v>173.36999499999999</v>
       </c>
-      <c r="D138">
+      <c r="D139" s="126">
         <f t="shared" si="11"/>
         <v>6.3228241913752425E-2</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="12">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="12">
         <v>44438</v>
       </c>
-      <c r="C139" s="18">
+      <c r="C140" s="18">
         <v>163.05999800000001</v>
       </c>
-      <c r="D139">
+      <c r="D140" s="126">
         <f t="shared" si="11"/>
         <v>0.3577019210275092</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="12">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="12">
         <v>44431</v>
       </c>
-      <c r="C140" s="18">
+      <c r="C141" s="18">
         <v>120.099998</v>
       </c>
-      <c r="D140">
+      <c r="D141" s="126">
         <f t="shared" si="11"/>
         <v>-4.7052297445467794E-2</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="12">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="12">
         <v>44424</v>
       </c>
-      <c r="C141" s="18">
+      <c r="C142" s="18">
         <v>126.029999</v>
       </c>
-      <c r="D141">
+      <c r="D142" s="126">
         <f t="shared" si="11"/>
         <v>-7.7581831311504423E-2</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="12">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="12">
         <v>44417</v>
       </c>
-      <c r="C142" s="18">
+      <c r="C143" s="18">
         <v>136.63000500000001</v>
       </c>
-      <c r="D142">
+      <c r="D143" s="126">
         <f t="shared" si="11"/>
         <v>1.6743562407219637E-2</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="12">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="12">
         <v>44410</v>
       </c>
-      <c r="C143" s="18">
+      <c r="C144" s="18">
         <v>134.38000500000001</v>
       </c>
-      <c r="D143">
+      <c r="D144" s="126">
         <f t="shared" si="11"/>
         <v>-4.1853796791443743E-2</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="12">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" s="12">
         <v>44403</v>
       </c>
-      <c r="C144" s="18">
+      <c r="C145" s="18">
         <v>140.25</v>
       </c>
     </row>

</xml_diff>